<commit_message>
Adding HumMod Data to Lab 26
</commit_message>
<xml_diff>
--- a/26_sodium_bicarbonate/sodium_bicarbonate_data.xlsx
+++ b/26_sodium_bicarbonate/sodium_bicarbonate_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>Time (Min)</t>
   </si>
@@ -37,6 +37,24 @@
   </si>
   <si>
     <t>Ventilation</t>
+  </si>
+  <si>
+    <t>UNITS</t>
+  </si>
+  <si>
+    <t>mmHg</t>
+  </si>
+  <si>
+    <t>L/min</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>For the HumMod version, the IV settings were an H2O rate of 100 mL/min with a bicarbonate concentration of 500 mmol/L</t>
   </si>
 </sst>
 </file>
@@ -58,15 +76,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -89,60 +113,24 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -438,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -449,7 +437,7 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,130 +456,330 @@
       <c r="F1" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>7.38</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>7.32</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>7.4</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>7.54</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <v>7.54</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="30.75" thickBot="1">
-      <c r="A3" s="3" t="s">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="30.75" thickBot="1">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>48</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>73</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>74</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>54</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A4" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>7.43</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>7.42</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <v>7.47</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>7.56</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <v>7.57</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="30.75" thickBot="1">
-      <c r="A5" s="3" t="s">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="30.75" thickBot="1">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>43</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>59</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>63</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>51</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A6" s="3" t="s">
+      <c r="G5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="2">
         <v>7.01</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>6.98</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>6.99</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>7.04</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>7.05</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A7" s="3" t="s">
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="2">
         <v>6.5</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>12.8</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>9.9</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="2">
         <v>4.5</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2">
+        <v>20</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2">
+        <v>7.38</v>
+      </c>
+      <c r="C11" s="2">
+        <v>7.55</v>
+      </c>
+      <c r="D11" s="2">
+        <v>7.65</v>
+      </c>
+      <c r="E11" s="2">
+        <v>7.73</v>
+      </c>
+      <c r="F11" s="2">
+        <v>7.79</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" ht="30.75" thickBot="1">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>41.6</v>
+      </c>
+      <c r="C12" s="2">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="D12" s="2">
+        <v>39.1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>38.6</v>
+      </c>
+      <c r="F12" s="2">
+        <v>37.9</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>7.43</v>
+      </c>
+      <c r="C13" s="2">
+        <v>7.58</v>
+      </c>
+      <c r="D13" s="2">
+        <v>7.68</v>
+      </c>
+      <c r="E13" s="2">
+        <v>7.75</v>
+      </c>
+      <c r="F13" s="2">
+        <v>7.81</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" ht="30.75" thickBot="1">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2">
+        <v>37.4</v>
+      </c>
+      <c r="C14" s="2">
+        <v>36.4</v>
+      </c>
+      <c r="D14" s="2">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="E14" s="2">
+        <v>36.5</v>
+      </c>
+      <c r="F14" s="2">
+        <v>36</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2">
+        <v>7.12</v>
+      </c>
+      <c r="C15" s="2">
+        <v>7.16</v>
+      </c>
+      <c r="D15" s="2">
+        <v>7.17</v>
+      </c>
+      <c r="E15" s="2">
+        <v>7.19</v>
+      </c>
+      <c r="F15" s="2">
+        <v>7.21</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2">
+        <v>6.6</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="E16" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A18:G19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding percentage differences to Lab 26
</commit_message>
<xml_diff>
--- a/26_sodium_bicarbonate/sodium_bicarbonate_data.xlsx
+++ b/26_sodium_bicarbonate/sodium_bicarbonate_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
   <si>
     <t>Time (Min)</t>
   </si>
@@ -61,7 +61,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +74,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -114,10 +121,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -132,9 +140,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -426,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -773,6 +785,192 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1"/>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>10</v>
+      </c>
+      <c r="E21" s="2">
+        <v>15</v>
+      </c>
+      <c r="F21" s="2">
+        <v>20</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="6">
+        <f>ABS((B2-B11)/B2)</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" ref="C22:F22" si="0">ABS((C2-C11)/C2)</f>
+        <v>3.1420765027322342E-2</v>
+      </c>
+      <c r="D22" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3783783783783779E-2</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="0"/>
+        <v>2.519893899204249E-2</v>
+      </c>
+      <c r="F22" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3156498673740056E-2</v>
+      </c>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="6">
+        <f t="shared" ref="B23:F23" si="1">ABS((B3-B12)/B3)</f>
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" si="1"/>
+        <v>0.4616438356164384</v>
+      </c>
+      <c r="D23" s="6">
+        <f t="shared" si="1"/>
+        <v>0.47162162162162158</v>
+      </c>
+      <c r="E23" s="6">
+        <f t="shared" si="1"/>
+        <v>0.28518518518518515</v>
+      </c>
+      <c r="F23" s="6">
+        <f t="shared" si="1"/>
+        <v>0.28490566037735854</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="6">
+        <f t="shared" ref="B24:F24" si="2">ABS((B4-B13)/B4)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" si="2"/>
+        <v>2.1563342318059318E-2</v>
+      </c>
+      <c r="D24" s="6">
+        <f t="shared" si="2"/>
+        <v>2.8112449799196783E-2</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" si="2"/>
+        <v>2.5132275132275186E-2</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" si="2"/>
+        <v>3.1704095112285245E-2</v>
+      </c>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="6">
+        <f t="shared" ref="B25:F25" si="3">ABS((B5-B14)/B5)</f>
+        <v>0.13023255813953491</v>
+      </c>
+      <c r="C25" s="6">
+        <f t="shared" si="3"/>
+        <v>0.38305084745762713</v>
+      </c>
+      <c r="D25" s="6">
+        <f t="shared" si="3"/>
+        <v>0.41746031746031742</v>
+      </c>
+      <c r="E25" s="6">
+        <f t="shared" si="3"/>
+        <v>0.28431372549019607</v>
+      </c>
+      <c r="F25" s="6">
+        <f t="shared" si="3"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="6">
+        <f t="shared" ref="B26:F26" si="4">ABS((B6-B15)/B6)</f>
+        <v>1.5691868758915879E-2</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" si="4"/>
+        <v>2.5787965616045804E-2</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="shared" si="4"/>
+        <v>2.5751072961373349E-2</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" si="4"/>
+        <v>2.1306818181818232E-2</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="4"/>
+        <v>2.269503546099293E-2</v>
+      </c>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="6">
+        <f t="shared" ref="B27:F27" si="5">ABS((B7-B16)/B7)</f>
+        <v>1.538461538461533E-2</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" si="5"/>
+        <v>0.67187500000000011</v>
+      </c>
+      <c r="D27" s="6">
+        <f t="shared" si="5"/>
+        <v>0.63636363636363646</v>
+      </c>
+      <c r="E27" s="6">
+        <f t="shared" si="5"/>
+        <v>0.23913043478260865</v>
+      </c>
+      <c r="F27" s="6">
+        <f t="shared" si="5"/>
+        <v>0.26666666666666672</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Adding colorcodes to Lab 26
</commit_message>
<xml_diff>
--- a/26_sodium_bicarbonate/sodium_bicarbonate_data.xlsx
+++ b/26_sodium_bicarbonate/sodium_bicarbonate_data.xlsx
@@ -134,21 +134,64 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -440,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -767,24 +810,24 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1"/>
     <row r="21" spans="1:7" ht="15.75" thickBot="1">
@@ -814,23 +857,23 @@
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="4">
         <f>ABS((B2-B11)/B2)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="4">
         <f t="shared" ref="C22:F22" si="0">ABS((C2-C11)/C2)</f>
         <v>3.1420765027322342E-2</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="4">
         <f t="shared" si="0"/>
         <v>3.3783783783783779E-2</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="4">
         <f t="shared" si="0"/>
         <v>2.519893899204249E-2</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="4">
         <f t="shared" si="0"/>
         <v>3.3156498673740056E-2</v>
       </c>
@@ -840,23 +883,23 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="4">
         <f t="shared" ref="B23:F23" si="1">ABS((B3-B12)/B3)</f>
         <v>0.1333333333333333</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="4">
         <f t="shared" si="1"/>
         <v>0.4616438356164384</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="4">
         <f t="shared" si="1"/>
         <v>0.47162162162162158</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="4">
         <f t="shared" si="1"/>
         <v>0.28518518518518515</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="4">
         <f t="shared" si="1"/>
         <v>0.28490566037735854</v>
       </c>
@@ -868,23 +911,23 @@
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="4">
         <f t="shared" ref="B24:F24" si="2">ABS((B4-B13)/B4)</f>
         <v>0</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="4">
         <f t="shared" si="2"/>
         <v>2.1563342318059318E-2</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="4">
         <f t="shared" si="2"/>
         <v>2.8112449799196783E-2</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="4">
         <f t="shared" si="2"/>
         <v>2.5132275132275186E-2</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="4">
         <f t="shared" si="2"/>
         <v>3.1704095112285245E-2</v>
       </c>
@@ -894,23 +937,23 @@
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="4">
         <f t="shared" ref="B25:F25" si="3">ABS((B5-B14)/B5)</f>
         <v>0.13023255813953491</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="4">
         <f t="shared" si="3"/>
         <v>0.38305084745762713</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="4">
         <f t="shared" si="3"/>
         <v>0.41746031746031742</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="4">
         <f t="shared" si="3"/>
         <v>0.28431372549019607</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="4">
         <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
@@ -922,23 +965,23 @@
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="4">
         <f t="shared" ref="B26:F26" si="4">ABS((B6-B15)/B6)</f>
         <v>1.5691868758915879E-2</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="4">
         <f t="shared" si="4"/>
         <v>2.5787965616045804E-2</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="4">
         <f t="shared" si="4"/>
         <v>2.5751072961373349E-2</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="4">
         <f t="shared" si="4"/>
         <v>2.1306818181818232E-2</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="4">
         <f t="shared" si="4"/>
         <v>2.269503546099293E-2</v>
       </c>
@@ -948,23 +991,23 @@
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="4">
         <f t="shared" ref="B27:F27" si="5">ABS((B7-B16)/B7)</f>
         <v>1.538461538461533E-2</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="4">
         <f t="shared" si="5"/>
         <v>0.67187500000000011</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="4">
         <f t="shared" si="5"/>
         <v>0.63636363636363646</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="4">
         <f t="shared" si="5"/>
         <v>0.23913043478260865</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="4">
         <f t="shared" si="5"/>
         <v>0.26666666666666672</v>
       </c>
@@ -976,6 +1019,15 @@
   <mergeCells count="1">
     <mergeCell ref="A18:G19"/>
   </mergeCells>
+  <conditionalFormatting sqref="B22:F27">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>